<commit_message>
Added Broken Links and Fluent Wait codes
</commit_message>
<xml_diff>
--- a/QuickTest/Resource/TestData.xlsx
+++ b/QuickTest/Resource/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>Praveen</t>
   </si>
@@ -377,8 +377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,12 +410,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>